<commit_message>
Chemistry Record plus more changes
</commit_message>
<xml_diff>
--- a/MS11/public_MS11.xlsx
+++ b/MS11/public_MS11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="375" windowWidth="17955" windowHeight="8730"/>
+    <workbookView xWindow="720" yWindow="375" windowWidth="14640" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,150 +805,169 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1">
-        <v>7508957390</v>
+        <v>8968066453</v>
       </c>
       <c r="C1">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>7837992019</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8427786799</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>9041564160</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8699367225</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9497278951</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>7837265544</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8606030818</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>9888213593</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>9815409350</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>9569902356</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9988153947</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9539267364</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>7696452043</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>9696438297</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8427786806</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="B7">
-        <v>8437789918</v>
+        <v>9530803331</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>9497455107</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B8">
-        <v>8968066453</v>
+        <v>9041847045</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -956,53 +975,59 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="B9">
-        <v>8968172389</v>
+        <v>7696211283</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B10">
-        <v>7837238536</v>
+        <v>9501518339</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>9902020656</v>
+        <v>7696452043</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11">
+        <v>9696438297</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1073,413 +1098,395 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16">
-        <v>8054297219</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" t="s">
-        <v>9</v>
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17">
-        <v>7837276673</v>
+        <v>122</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="H17" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>126</v>
+      </c>
+      <c r="B18">
+        <v>9814739262</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="H18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="B19">
-        <v>8699429869</v>
+        <v>9855588551</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="H19" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20">
-        <v>8054650066</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21">
-        <v>7508855158</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
+      <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8968033297</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22">
-        <v>9872317665</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="2">
+        <v>9914773168</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B23">
-        <v>9646947488</v>
+        <v>9646970307</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>8872880424</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B24">
-        <v>8427996449</v>
+        <v>9041564160</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="B25">
-        <v>8054324817</v>
+        <v>7837265544</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <v>9988260454</v>
+        <v>8437789918</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
-        <v>34</v>
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>8054297219</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2">
-        <v>9646172958</v>
+        <v>9041564154</v>
       </c>
       <c r="C28" s="2">
         <v>2</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>9041658278</v>
+        <v>7508988823</v>
       </c>
       <c r="C29" s="2">
         <v>2</v>
       </c>
       <c r="D29" s="2">
-        <v>8699169761</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>8699739672</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2">
-        <v>8427786799</v>
+        <v>9888119037</v>
       </c>
       <c r="C30" s="2">
         <v>2</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>62</v>
+      <c r="E30" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2">
-        <v>8699367225</v>
+        <v>9646938448</v>
       </c>
       <c r="C31" s="2">
         <v>2</v>
       </c>
-      <c r="D31" s="2">
-        <v>9497278951</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="2">
-        <v>8968159116</v>
-      </c>
-      <c r="C32" s="2">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32">
+        <v>9041657730</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="2">
-        <v>9041564154</v>
-      </c>
-      <c r="C33" s="2">
-        <v>2</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H33" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="I33" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="2">
-        <v>8968033297</v>
-      </c>
-      <c r="C34" s="2">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="A34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34">
+        <v>7696443696</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="2">
-        <v>7508988823</v>
-      </c>
-      <c r="C35" s="2">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2">
-        <v>8699739672</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>7837992019</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="2">
-        <v>8699341657</v>
-      </c>
-      <c r="C36" s="2">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>7837238536</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1503,49 +1510,51 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2">
-        <v>8699431031</v>
+        <v>8146894390</v>
       </c>
       <c r="C38" s="2">
         <v>2</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B39" s="2">
-        <v>9888119037</v>
+        <v>7696443610</v>
       </c>
       <c r="C39" s="2">
         <v>2</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="3" t="s">
-        <v>73</v>
+      <c r="E39" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
@@ -1556,7 +1565,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
@@ -1564,510 +1573,461 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="2">
-        <v>8146894390</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2" t="s">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41">
+        <v>7696399642</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
         <v>5</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="2">
-        <v>9646938448</v>
-      </c>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42">
+        <v>7307310635</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="2">
-        <v>8968769989</v>
-      </c>
-      <c r="C43" s="2">
-        <v>2</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43">
+        <v>9646642757</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="2">
-        <v>9914773168</v>
-      </c>
-      <c r="C44" s="2">
-        <v>2</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="A44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44">
+        <v>9876110998</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H44" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="2">
-        <v>7696443610</v>
-      </c>
-      <c r="C45" s="2">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2" t="s">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45">
+        <v>9501157243</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" t="s">
         <v>5</v>
       </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="2">
-        <v>7696193723</v>
-      </c>
-      <c r="C46" s="2">
-        <v>2</v>
-      </c>
-      <c r="D46" s="2">
-        <v>7696193723</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46">
+        <v>8968172389</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47">
+        <v>9902020656</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="2">
-        <v>8872808043</v>
-      </c>
-      <c r="C47" s="2">
-        <v>2</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48">
+        <v>8054650066</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H48" t="s">
         <v>24</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="2">
-        <v>8606030818</v>
-      </c>
-      <c r="C48" s="2">
-        <v>2</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="2">
-        <v>9988153947</v>
-      </c>
-      <c r="C49" s="2">
-        <v>2</v>
-      </c>
-      <c r="D49" s="2">
-        <v>9539267364</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>7508855158</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="2">
-        <v>8427786806</v>
-      </c>
-      <c r="C50" s="2">
-        <v>2</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>9872317665</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2">
-        <v>2</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2" t="s">
-        <v>34</v>
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>9646947488</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H51" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="2">
-        <v>9646471963</v>
-      </c>
-      <c r="C52" s="2">
-        <v>2</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>8054324817</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H52" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>9530803331</v>
+        <v>9988260454</v>
       </c>
       <c r="C53">
-        <v>3</v>
-      </c>
-      <c r="D53">
-        <v>9497455107</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="H53" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54">
-        <v>7696399642</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="H54" t="s">
-        <v>5</v>
-      </c>
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2">
+        <v>9646172958</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55">
-        <v>9041847045</v>
-      </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H55" t="s">
-        <v>21</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="2">
+        <v>8968159116</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56">
-        <v>8765653385</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" t="s">
-        <v>102</v>
-      </c>
+      <c r="A56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="2">
+        <v>8699431031</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57">
-        <v>7307310635</v>
-      </c>
-      <c r="C57">
-        <v>3</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H57" t="s">
-        <v>5</v>
-      </c>
+      <c r="A57" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="2">
+        <v>8872808043</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58">
-        <v>7696211283</v>
+        <v>134</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="E58" s="1"/>
       <c r="H58" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="J58" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B59">
-        <v>9041003765</v>
+        <v>8765653385</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>108</v>
+      <c r="E59" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="H59" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60">
-        <v>9501518339</v>
+        <v>123</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="H60" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
-      </c>
-      <c r="B61">
-        <v>7589489022</v>
+        <v>128</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="H61" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62">
-        <v>9041657730</v>
+        <v>102</v>
       </c>
       <c r="C62">
         <v>3</v>
       </c>
+      <c r="E62" s="1"/>
       <c r="H62" t="s">
-        <v>9</v>
+        <v>102</v>
+      </c>
+      <c r="J62" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="B63">
-        <v>9646642757</v>
+        <v>7508957390</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>9888213593</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>9815409350</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>116</v>
+        <v>13</v>
+      </c>
+      <c r="F64">
+        <v>9569902356</v>
       </c>
       <c r="H64" t="s">
-        <v>9</v>
-      </c>
-      <c r="I64" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="B65">
-        <v>9876110998</v>
+        <v>7837276673</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="H65" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>119</v>
-      </c>
-      <c r="B66">
-        <v>7696443696</v>
+        <v>40</v>
       </c>
       <c r="C66">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E66" s="1"/>
       <c r="H66" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="J66" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B67">
-        <v>8960330251</v>
+        <v>8699429869</v>
       </c>
       <c r="C67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="H67" t="s">
         <v>2</v>
@@ -2075,136 +2035,177 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>51</v>
+      </c>
+      <c r="B68">
+        <v>8427996449</v>
       </c>
       <c r="C68">
-        <v>3</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="H68" t="s">
-        <v>16</v>
-      </c>
-      <c r="J68" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>123</v>
-      </c>
-      <c r="C69">
-        <v>3</v>
-      </c>
-      <c r="H69" t="s">
-        <v>102</v>
-      </c>
+      <c r="A69" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="2">
+        <v>9041658278</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2</v>
+      </c>
+      <c r="D69" s="2">
+        <v>8699169761</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69" s="2"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>124</v>
-      </c>
-      <c r="B70">
-        <v>9501157243</v>
-      </c>
-      <c r="C70">
-        <v>3</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H70" t="s">
-        <v>5</v>
-      </c>
+      <c r="A70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2">
+        <v>8699341657</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71">
-        <v>9814739262</v>
-      </c>
-      <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H71" t="s">
-        <v>16</v>
-      </c>
+      <c r="A71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="2">
+        <v>8968769989</v>
+      </c>
+      <c r="C71" s="2">
+        <v>2</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="H72" t="s">
-        <v>102</v>
-      </c>
+      <c r="A72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="2">
+        <v>7696193723</v>
+      </c>
+      <c r="C72" s="2">
+        <v>2</v>
+      </c>
+      <c r="D72" s="2">
+        <v>7696193723</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73">
-        <v>9646970307</v>
-      </c>
-      <c r="C73">
-        <v>3</v>
-      </c>
-      <c r="D73">
-        <v>8872880424</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H73" t="s">
-        <v>58</v>
-      </c>
+      <c r="A73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="2">
+        <v>9646471963</v>
+      </c>
+      <c r="C73" s="2">
+        <v>2</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B74">
-        <v>9855588551</v>
+        <v>9041003765</v>
       </c>
       <c r="C74">
         <v>3</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>132</v>
+      <c r="G74" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="H74" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>111</v>
+      </c>
+      <c r="B75">
+        <v>7589489022</v>
       </c>
       <c r="C75">
         <v>3</v>
       </c>
-      <c r="E75" s="1"/>
+      <c r="E75" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="H75" t="s">
-        <v>102</v>
-      </c>
-      <c r="J75" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B76">
-        <v>9569975642</v>
+        <v>8960330251</v>
       </c>
       <c r="C76">
         <v>3</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="H76" t="s">
         <v>2</v>
@@ -2212,76 +2213,78 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="B77">
+        <v>9569975642</v>
       </c>
       <c r="C77">
         <v>3</v>
       </c>
-      <c r="E77" s="1"/>
       <c r="H77" t="s">
-        <v>24</v>
-      </c>
-      <c r="J77" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:J77">
+    <sortCondition ref="H1:H77"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E53" r:id="rId1"/>
-    <hyperlink ref="E1" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E5" r:id="rId5"/>
-    <hyperlink ref="E17" r:id="rId6"/>
-    <hyperlink ref="E19" r:id="rId7"/>
-    <hyperlink ref="E6" r:id="rId8"/>
-    <hyperlink ref="E22" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E31" r:id="rId11"/>
-    <hyperlink ref="E49" r:id="rId12"/>
-    <hyperlink ref="E60" r:id="rId13"/>
-    <hyperlink ref="E50" r:id="rId14"/>
-    <hyperlink ref="G59" r:id="rId15"/>
-    <hyperlink ref="E58" r:id="rId16"/>
-    <hyperlink ref="E7" r:id="rId17"/>
-    <hyperlink ref="E8" r:id="rId18"/>
-    <hyperlink ref="E48" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E26" r:id="rId21"/>
-    <hyperlink ref="E33" r:id="rId22"/>
-    <hyperlink ref="E64" r:id="rId23"/>
-    <hyperlink ref="E16" r:id="rId24"/>
-    <hyperlink ref="E28" r:id="rId25"/>
-    <hyperlink ref="E47" r:id="rId26"/>
-    <hyperlink ref="E55" r:id="rId27"/>
-    <hyperlink ref="E30" r:id="rId28"/>
-    <hyperlink ref="E56" r:id="rId29"/>
-    <hyperlink ref="E71" r:id="rId30"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E63" r:id="rId2"/>
+    <hyperlink ref="E24" r:id="rId3"/>
+    <hyperlink ref="E25" r:id="rId4"/>
+    <hyperlink ref="E64" r:id="rId5"/>
+    <hyperlink ref="E65" r:id="rId6"/>
+    <hyperlink ref="E67" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E50" r:id="rId9"/>
+    <hyperlink ref="E47" r:id="rId10"/>
+    <hyperlink ref="E3" r:id="rId11"/>
+    <hyperlink ref="E5" r:id="rId12"/>
+    <hyperlink ref="E10" r:id="rId13"/>
+    <hyperlink ref="E6" r:id="rId14"/>
+    <hyperlink ref="G74" r:id="rId15"/>
+    <hyperlink ref="E9" r:id="rId16"/>
+    <hyperlink ref="E26" r:id="rId17"/>
+    <hyperlink ref="E1" r:id="rId18"/>
+    <hyperlink ref="E4" r:id="rId19"/>
+    <hyperlink ref="E49" r:id="rId20"/>
+    <hyperlink ref="E53" r:id="rId21"/>
+    <hyperlink ref="E28" r:id="rId22"/>
+    <hyperlink ref="E33" r:id="rId23"/>
+    <hyperlink ref="E27" r:id="rId24"/>
+    <hyperlink ref="E54" r:id="rId25"/>
+    <hyperlink ref="E57" r:id="rId26"/>
+    <hyperlink ref="E8" r:id="rId27"/>
+    <hyperlink ref="E2" r:id="rId28"/>
+    <hyperlink ref="E59" r:id="rId29"/>
+    <hyperlink ref="E18" r:id="rId30"/>
     <hyperlink ref="E12" r:id="rId31"/>
-    <hyperlink ref="E74" r:id="rId32"/>
-    <hyperlink ref="E44" r:id="rId33"/>
-    <hyperlink ref="E73" r:id="rId34"/>
-    <hyperlink ref="E32" r:id="rId35"/>
-    <hyperlink ref="E20" r:id="rId36"/>
-    <hyperlink ref="E25" r:id="rId37"/>
-    <hyperlink ref="E23" r:id="rId38"/>
-    <hyperlink ref="E24" r:id="rId39"/>
-    <hyperlink ref="E42" r:id="rId40"/>
-    <hyperlink ref="E41" r:id="rId41"/>
-    <hyperlink ref="E46" r:id="rId42"/>
-    <hyperlink ref="E57" r:id="rId43"/>
-    <hyperlink ref="E61" r:id="rId44"/>
-    <hyperlink ref="E65" r:id="rId45"/>
-    <hyperlink ref="E67" r:id="rId46"/>
-    <hyperlink ref="E70" r:id="rId47"/>
-    <hyperlink ref="E2" r:id="rId48"/>
-    <hyperlink ref="E10" r:id="rId49"/>
-    <hyperlink ref="E43" r:id="rId50"/>
+    <hyperlink ref="E19" r:id="rId32"/>
+    <hyperlink ref="E22" r:id="rId33"/>
+    <hyperlink ref="E23" r:id="rId34"/>
+    <hyperlink ref="E55" r:id="rId35"/>
+    <hyperlink ref="E48" r:id="rId36"/>
+    <hyperlink ref="E52" r:id="rId37"/>
+    <hyperlink ref="E51" r:id="rId38"/>
+    <hyperlink ref="E68" r:id="rId39"/>
+    <hyperlink ref="E31" r:id="rId40"/>
+    <hyperlink ref="E38" r:id="rId41"/>
+    <hyperlink ref="E72" r:id="rId42"/>
+    <hyperlink ref="E42" r:id="rId43"/>
+    <hyperlink ref="E75" r:id="rId44"/>
+    <hyperlink ref="E44" r:id="rId45"/>
+    <hyperlink ref="E76" r:id="rId46"/>
+    <hyperlink ref="E45" r:id="rId47"/>
+    <hyperlink ref="E35" r:id="rId48"/>
+    <hyperlink ref="E36" r:id="rId49"/>
+    <hyperlink ref="E71" r:id="rId50"/>
     <hyperlink ref="E13" r:id="rId51"/>
-    <hyperlink ref="E45" r:id="rId52"/>
-    <hyperlink ref="E9" r:id="rId53"/>
-    <hyperlink ref="E35" r:id="rId54"/>
-    <hyperlink ref="E39" r:id="rId55"/>
+    <hyperlink ref="E39" r:id="rId52"/>
+    <hyperlink ref="E46" r:id="rId53"/>
+    <hyperlink ref="E29" r:id="rId54"/>
+    <hyperlink ref="E30" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hell lot of changes and additions :)
</commit_message>
<xml_diff>
--- a/MS11/public_MS11.xlsx
+++ b/MS11/public_MS11.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A. S. Aurora\Documents\IISER_repo\MS11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="375" windowWidth="14640" windowHeight="8355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="List" sheetId="1" r:id="rId1"/>
+    <sheet name="Ankita" sheetId="8" r:id="rId2"/>
+    <sheet name="Shwetha" sheetId="7" r:id="rId3"/>
+    <sheet name="Amritha" sheetId="2" r:id="rId4"/>
+    <sheet name="Arpit" sheetId="3" r:id="rId5"/>
+    <sheet name="Manisha" sheetId="4" r:id="rId6"/>
+    <sheet name="Manu J" sheetId="5" r:id="rId7"/>
+    <sheet name="Arjit" sheetId="6" r:id="rId8"/>
+    <sheet name="Yashpal" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="139">
   <si>
     <t>Abhinav</t>
   </si>
@@ -421,6 +432,18 @@
   </si>
   <si>
     <t>Yosman</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -464,10 +487,36 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -478,11 +527,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -494,6 +546,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -542,7 +597,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -577,7 +632,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -788,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
@@ -1485,7 +1540,7 @@
         <v>26</v>
       </c>
       <c r="H36" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1502,8 +1557,8 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2" t="s">
-        <v>5</v>
+      <c r="H37" t="s">
+        <v>103</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1524,8 +1579,8 @@
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2" t="s">
-        <v>5</v>
+      <c r="H38" t="s">
+        <v>103</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1546,8 +1601,8 @@
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2" t="s">
-        <v>5</v>
+      <c r="H39" t="s">
+        <v>103</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -1556,7 +1611,9 @@
       <c r="A40" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>9530846804</v>
+      </c>
       <c r="C40" s="2">
         <v>2</v>
       </c>
@@ -1564,8 +1621,8 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
-        <v>5</v>
+      <c r="H40" t="s">
+        <v>103</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
@@ -1583,7 +1640,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1600,7 +1657,7 @@
         <v>104</v>
       </c>
       <c r="H42" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1614,7 +1671,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1631,7 +1688,7 @@
         <v>118</v>
       </c>
       <c r="H44" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1648,7 +1705,7 @@
         <v>125</v>
       </c>
       <c r="H45" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2287,29 +2344,1724 @@
     <hyperlink ref="E30" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId56"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major changes, chemistry and workshop completed
</commit_message>
<xml_diff>
--- a/MS11/public_MS11.xlsx
+++ b/MS11/public_MS11.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F2" s="2"/>
@@ -2353,7 +2353,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3774,7 +3774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>